<commit_message>
fix it completed for 10 lessons
</commit_message>
<xml_diff>
--- a/public/docs/Grammar_fixit_exercise.xlsx
+++ b/public/docs/Grammar_fixit_exercise.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7B1BF6-9C5C-4874-B257-2F503190C0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E52A4EE-FA00-4DF6-94C7-848985C22154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="1104" windowWidth="13512" windowHeight="8880" xr2:uid="{957858FE-AC4D-42E8-AFE4-77BBB2FEBAB6}"/>
+    <workbookView xWindow="1080" yWindow="1800" windowWidth="13512" windowHeight="8880" xr2:uid="{957858FE-AC4D-42E8-AFE4-77BBB2FEBAB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2684" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2582" uniqueCount="256">
   <si>
     <t>{beginning: "</t>
   </si>
@@ -369,6 +370,441 @@
   </si>
   <si>
     <t>the new project</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>ended</t>
+  </si>
+  <si>
+    <t>the meeting</t>
+  </si>
+  <si>
+    <t>follow</t>
+  </si>
+  <si>
+    <t>followed</t>
+  </si>
+  <si>
+    <t>the new method</t>
+  </si>
+  <si>
+    <t>He never</t>
+  </si>
+  <si>
+    <t>imagine</t>
+  </si>
+  <si>
+    <t>imagined</t>
+  </si>
+  <si>
+    <t>such a result</t>
+  </si>
+  <si>
+    <t>use</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>less water last week</t>
+  </si>
+  <si>
+    <t>The children</t>
+  </si>
+  <si>
+    <t>play</t>
+  </si>
+  <si>
+    <t>played</t>
+  </si>
+  <si>
+    <t>in the yard all day</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>was</t>
+  </si>
+  <si>
+    <t>able to the finish the project</t>
+  </si>
+  <si>
+    <t>clime</t>
+  </si>
+  <si>
+    <t>climed</t>
+  </si>
+  <si>
+    <t>the hilltop</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>pointed</t>
+  </si>
+  <si>
+    <t>at the map</t>
+  </si>
+  <si>
+    <t>bring</t>
+  </si>
+  <si>
+    <t>brought</t>
+  </si>
+  <si>
+    <t>her book</t>
+  </si>
+  <si>
+    <t>choose</t>
+  </si>
+  <si>
+    <t>chose</t>
+  </si>
+  <si>
+    <t>the red shirt</t>
+  </si>
+  <si>
+    <t>come</t>
+  </si>
+  <si>
+    <t>came</t>
+  </si>
+  <si>
+    <t>to the concert late</t>
+  </si>
+  <si>
+    <t>drink</t>
+  </si>
+  <si>
+    <t>drank</t>
+  </si>
+  <si>
+    <t>a glass of water</t>
+  </si>
+  <si>
+    <t>drive</t>
+  </si>
+  <si>
+    <t>drove</t>
+  </si>
+  <si>
+    <t>to the city</t>
+  </si>
+  <si>
+    <t>The bird</t>
+  </si>
+  <si>
+    <t>fly</t>
+  </si>
+  <si>
+    <t>flew</t>
+  </si>
+  <si>
+    <t>over the trees</t>
+  </si>
+  <si>
+    <t>forget</t>
+  </si>
+  <si>
+    <t>forgot</t>
+  </si>
+  <si>
+    <t>to do his homework</t>
+  </si>
+  <si>
+    <t>gave</t>
+  </si>
+  <si>
+    <t>me a nice gift</t>
+  </si>
+  <si>
+    <t>The girl</t>
+  </si>
+  <si>
+    <t>get (past)</t>
+  </si>
+  <si>
+    <t>did not get</t>
+  </si>
+  <si>
+    <t>the job</t>
+  </si>
+  <si>
+    <t>play (future)</t>
+  </si>
+  <si>
+    <t>will not play</t>
+  </si>
+  <si>
+    <t>at the party</t>
+  </si>
+  <si>
+    <t>meet (present)</t>
+  </si>
+  <si>
+    <t>do not meet</t>
+  </si>
+  <si>
+    <t>every day</t>
+  </si>
+  <si>
+    <t>understand (past)</t>
+  </si>
+  <si>
+    <t>did not understand</t>
+  </si>
+  <si>
+    <t>the question</t>
+  </si>
+  <si>
+    <t>stop (future)</t>
+  </si>
+  <si>
+    <t>will not stop</t>
+  </si>
+  <si>
+    <t>there</t>
+  </si>
+  <si>
+    <t>does not bring</t>
+  </si>
+  <si>
+    <t>the books to school</t>
+  </si>
+  <si>
+    <t>read (past)</t>
+  </si>
+  <si>
+    <t>did not read</t>
+  </si>
+  <si>
+    <t>the message carefully</t>
+  </si>
+  <si>
+    <t>arrive (future)</t>
+  </si>
+  <si>
+    <t>will not arrive</t>
+  </si>
+  <si>
+    <t>for the meeting</t>
+  </si>
+  <si>
+    <t>stay</t>
+  </si>
+  <si>
+    <t>were staying</t>
+  </si>
+  <si>
+    <t>at home all weekend</t>
+  </si>
+  <si>
+    <t>feel</t>
+  </si>
+  <si>
+    <t>was feeling</t>
+  </si>
+  <si>
+    <t>bad about his decision</t>
+  </si>
+  <si>
+    <t>was eating</t>
+  </si>
+  <si>
+    <t>the cake when they arrived</t>
+  </si>
+  <si>
+    <t>discuss</t>
+  </si>
+  <si>
+    <t>were discussing</t>
+  </si>
+  <si>
+    <t>the theory in the class</t>
+  </si>
+  <si>
+    <t>prepare</t>
+  </si>
+  <si>
+    <t>was preparing</t>
+  </si>
+  <si>
+    <t>dinner for her friends</t>
+  </si>
+  <si>
+    <t>The students</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>were studying</t>
+  </si>
+  <si>
+    <t>law all evening</t>
+  </si>
+  <si>
+    <t>cook</t>
+  </si>
+  <si>
+    <t>was cooking</t>
+  </si>
+  <si>
+    <t>food when I called</t>
+  </si>
+  <si>
+    <t>The boys</t>
+  </si>
+  <si>
+    <t>put</t>
+  </si>
+  <si>
+    <t>were putting</t>
+  </si>
+  <si>
+    <t>the books on the shelf</t>
+  </si>
+  <si>
+    <t>sing (past)</t>
+  </si>
+  <si>
+    <t>was not singing</t>
+  </si>
+  <si>
+    <t>in the morning</t>
+  </si>
+  <si>
+    <t>The guide</t>
+  </si>
+  <si>
+    <t>explain (present)</t>
+  </si>
+  <si>
+    <t>is not explaining</t>
+  </si>
+  <si>
+    <t>it clearly</t>
+  </si>
+  <si>
+    <t>provide (future)</t>
+  </si>
+  <si>
+    <t>will not be providing</t>
+  </si>
+  <si>
+    <t>enough information</t>
+  </si>
+  <si>
+    <t>change (past)</t>
+  </si>
+  <si>
+    <t>was not changing</t>
+  </si>
+  <si>
+    <t>her opinion</t>
+  </si>
+  <si>
+    <t>show (future)</t>
+  </si>
+  <si>
+    <t>will not be showing</t>
+  </si>
+  <si>
+    <t>interest in this topic</t>
+  </si>
+  <si>
+    <t>study (present)</t>
+  </si>
+  <si>
+    <t>are not studying</t>
+  </si>
+  <si>
+    <t>literature at this lesson</t>
+  </si>
+  <si>
+    <t>visit (past)</t>
+  </si>
+  <si>
+    <t>was not visiting</t>
+  </si>
+  <si>
+    <t>them last month</t>
+  </si>
+  <si>
+    <t>solve (future)</t>
+  </si>
+  <si>
+    <t>will not be solving</t>
+  </si>
+  <si>
+    <t>the problem correctly</t>
+  </si>
+  <si>
+    <t>has not found</t>
+  </si>
+  <si>
+    <t>her card</t>
+  </si>
+  <si>
+    <t>face</t>
+  </si>
+  <si>
+    <t>have not faced</t>
+  </si>
+  <si>
+    <t>any difficulties so far</t>
+  </si>
+  <si>
+    <t>include</t>
+  </si>
+  <si>
+    <t>have not included</t>
+  </si>
+  <si>
+    <t>Sarah in the list</t>
+  </si>
+  <si>
+    <t>has not made</t>
+  </si>
+  <si>
+    <t>a list of items to buy</t>
+  </si>
+  <si>
+    <t>have not changed</t>
+  </si>
+  <si>
+    <t>my mind about the trip</t>
+  </si>
+  <si>
+    <t>mention</t>
+  </si>
+  <si>
+    <t>has not mentioned</t>
+  </si>
+  <si>
+    <t>any reason</t>
+  </si>
+  <si>
+    <t>see</t>
+  </si>
+  <si>
+    <t>have not seen</t>
+  </si>
+  <si>
+    <t>the real problem yet</t>
+  </si>
+  <si>
+    <t>try</t>
+  </si>
+  <si>
+    <t>have not tried</t>
+  </si>
+  <si>
+    <t>various solutions yet</t>
   </si>
 </sst>
 </file>
@@ -776,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB64D9CB-62E1-4E7F-A9F1-9B1326169423}">
-  <dimension ref="A2:J358"/>
+  <dimension ref="A2:J346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H35" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39:J46"/>
+    <sheetView tabSelected="1" topLeftCell="I96" workbookViewId="0">
+      <selection activeCell="J99" sqref="J99:J106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2074,30 +2510,33 @@
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B49" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="C49" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>9</v>
+        <v>112</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>10</v>
+        <v>113</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J49" s="2" t="str">
         <f>A49&amp;B49&amp;C49&amp;D49&amp;E49&amp;F49&amp;G49&amp;H49&amp;I49</f>
-        <v>{beginning: "", bold: "Я", correct: "I", ending: "love Ukraine"},</v>
+        <v>{beginning: "They", bold: "end", correct: "ended", ending: "the meeting"},</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
@@ -2105,32 +2544,32 @@
         <v>0</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>2</v>
+        <v>115</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J50" s="2" t="str">
         <f>A50&amp;B50&amp;C50&amp;D50&amp;E50&amp;F50&amp;G50&amp;H50&amp;I50</f>
-        <v>{beginning: "beginning text", bold: "word text2", correct: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She", bold: "follow", correct: "followed", ending: "the new method"},</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -2138,32 +2577,32 @@
         <v>0</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>11</v>
+        <v>118</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>4</v>
+        <v>120</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J51" s="2" t="str">
-        <f t="shared" ref="J51:J58" si="4">A51&amp;B51&amp;C51&amp;D51&amp;E51&amp;F51&amp;G51&amp;H51&amp;I51</f>
-        <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" ref="J51:J56" si="4">A51&amp;B51&amp;C51&amp;D51&amp;E51&amp;F51&amp;G51&amp;H51&amp;I51</f>
+        <v>{beginning: "He never", bold: "imagine", correct: "imagined", ending: "such a result"},</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -2171,32 +2610,32 @@
         <v>0</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>2</v>
+        <v>122</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>4</v>
+        <v>123</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J52" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "We", bold: "use", correct: "used", ending: "less water last week"},</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -2204,32 +2643,32 @@
         <v>0</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>2</v>
+        <v>126</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>4</v>
+        <v>127</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J53" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "The children", bold: "play", correct: "played", ending: "in the yard all day"},</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
@@ -2237,32 +2676,32 @@
         <v>0</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>14</v>
+        <v>128</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>2</v>
+        <v>129</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>4</v>
+        <v>130</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J54" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She", bold: "be", correct: "was", ending: "able to the finish the project"},</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -2270,32 +2709,32 @@
         <v>0</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>4</v>
+        <v>133</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J55" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "They", bold: "clime", correct: "climed", ending: "the hilltop"},</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -2303,133 +2742,136 @@
         <v>0</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>16</v>
+        <v>134</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>2</v>
+        <v>135</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J56" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J57" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He", bold: "point", correct: "pointed", ending: "at the map"},</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J58" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
+      <c r="A58" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J59" s="2" t="str">
+        <f>A59&amp;B59&amp;C59&amp;D59&amp;E59&amp;F59&amp;G59&amp;H59&amp;I59</f>
+        <v>{beginning: "She", bold: "bring", correct: "brought", ending: "her book"},</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
-        <v>23</v>
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J60" s="2" t="str">
+        <f>A60&amp;B60&amp;C60&amp;D60&amp;E60&amp;F60&amp;G60&amp;H60&amp;I60</f>
+        <v>{beginning: "He", bold: "choose", correct: "chose", ending: "the red shirt"},</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B61" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="C61" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>8</v>
+        <v>143</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>10</v>
+        <v>145</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J61" s="2" t="str">
-        <f>A61&amp;B61&amp;C61&amp;D61&amp;E61&amp;F61&amp;G61&amp;H61&amp;I61</f>
-        <v>{beginning: "", bold: "Я", correct: "I", ending: "love Ukraine"},</v>
+        <f t="shared" ref="J61:J66" si="5">A61&amp;B61&amp;C61&amp;D61&amp;E61&amp;F61&amp;G61&amp;H61&amp;I61</f>
+        <v>{beginning: "They", bold: "come", correct: "came", ending: "to the concert late"},</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
@@ -2437,32 +2879,32 @@
         <v>0</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>2</v>
+        <v>147</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>4</v>
+        <v>148</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J62" s="2" t="str">
-        <f>A62&amp;B62&amp;C62&amp;D62&amp;E62&amp;F62&amp;G62&amp;H62&amp;I62</f>
-        <v>{beginning: "beginning text", bold: "word text2", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="5"/>
+        <v>{beginning: "I", bold: "drink", correct: "drank", ending: "a glass of water"},</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -2470,32 +2912,32 @@
         <v>0</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>11</v>
+        <v>149</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>2</v>
+        <v>150</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>4</v>
+        <v>151</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J63" s="2" t="str">
-        <f t="shared" ref="J63:J70" si="5">A63&amp;B63&amp;C63&amp;D63&amp;E63&amp;F63&amp;G63&amp;H63&amp;I63</f>
-        <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="5"/>
+        <v>{beginning: "We", bold: "drive", correct: "drove", ending: "to the city"},</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
@@ -2503,32 +2945,32 @@
         <v>0</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>2</v>
+        <v>154</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>4</v>
+        <v>155</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J64" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "The bird", bold: "fly", correct: "flew", ending: "over the trees"},</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
@@ -2536,32 +2978,32 @@
         <v>0</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>13</v>
+        <v>156</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>2</v>
+        <v>157</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>4</v>
+        <v>158</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J65" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He", bold: "forget", correct: "forgot", ending: "to do his homework"},</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
@@ -2569,98 +3011,37 @@
         <v>0</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>2</v>
+        <v>159</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J66" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J67" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "She", bold: "give", correct: "gave", ending: "me a nice gift"},</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J68" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
+      <c r="A68" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
@@ -2668,32 +3049,32 @@
         <v>0</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>17</v>
+        <v>162</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>2</v>
+        <v>163</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J69" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
+        <f>A69&amp;B69&amp;C69&amp;D69&amp;E69&amp;F69&amp;G69&amp;H69&amp;I69</f>
+        <v>{beginning: "The girl", bold: "get (past)", correct: "did not get", ending: "the job"},</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
@@ -2701,67 +3082,131 @@
         <v>0</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>18</v>
+        <v>165</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>2</v>
+        <v>166</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>4</v>
+        <v>167</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J70" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
+        <f>A70&amp;B70&amp;C70&amp;D70&amp;E70&amp;F70&amp;G70&amp;H70&amp;I70</f>
+        <v>{beginning: "They", bold: "play (future)", correct: "will not play", ending: "at the party"},</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J71" s="2" t="str">
+        <f t="shared" ref="J71:J76" si="6">A71&amp;B71&amp;C71&amp;D71&amp;E71&amp;F71&amp;G71&amp;H71&amp;I71</f>
+        <v>{beginning: "He", bold: "meet (present)", correct: "do not meet", ending: "every day"},</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A72" s="4" t="s">
-        <v>24</v>
+      <c r="A72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J72" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>{beginning: "I", bold: "understand (past)", correct: "did not understand", ending: "the question"},</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B73" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C73" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>8</v>
+        <v>174</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>9</v>
+        <v>175</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>10</v>
+        <v>176</v>
       </c>
       <c r="I73" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J73" s="2" t="str">
-        <f>A73&amp;B73&amp;C73&amp;D73&amp;E73&amp;F73&amp;G73&amp;H73&amp;I73</f>
-        <v>{beginning: "", bold: "Я", correct: "I", ending: "love Ukraine"},</v>
+        <f t="shared" si="6"/>
+        <v>{beginning: "We", bold: "stop (future)", correct: "will not stop", ending: "there"},</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
@@ -2769,32 +3214,32 @@
         <v>0</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>6</v>
+        <v>137</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>2</v>
+        <v>177</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>4</v>
+        <v>178</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J74" s="2" t="str">
-        <f>A74&amp;B74&amp;C74&amp;D74&amp;E74&amp;F74&amp;G74&amp;H74&amp;I74</f>
-        <v>{beginning: "beginning text", bold: "word text2", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="6"/>
+        <v>{beginning: "She", bold: "bring", correct: "does not bring", ending: "the books to school"},</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
@@ -2802,32 +3247,32 @@
         <v>0</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>11</v>
+        <v>179</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>2</v>
+        <v>180</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>4</v>
+        <v>181</v>
       </c>
       <c r="I75" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J75" s="2" t="str">
-        <f t="shared" ref="J75:J82" si="6">A75&amp;B75&amp;C75&amp;D75&amp;E75&amp;F75&amp;G75&amp;H75&amp;I75</f>
-        <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="6"/>
+        <v>{beginning: "I", bold: "read (past)", correct: "did not read", ending: "the message carefully"},</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
@@ -2835,98 +3280,37 @@
         <v>0</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>12</v>
+        <v>182</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>2</v>
+        <v>183</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>4</v>
+        <v>184</v>
       </c>
       <c r="I76" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J76" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J77" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
+        <v>{beginning: "He", bold: "arrive (future)", correct: "will not arrive", ending: "for the meeting"},</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H78" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I78" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J78" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
+      <c r="A78" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
@@ -2934,32 +3318,32 @@
         <v>0</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>15</v>
+        <v>185</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>2</v>
+        <v>186</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>4</v>
+        <v>187</v>
       </c>
       <c r="I79" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J79" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
+        <f>A79&amp;B79&amp;C79&amp;D79&amp;E79&amp;F79&amp;G79&amp;H79&amp;I79</f>
+        <v>{beginning: "They", bold: "stay", correct: "were staying", ending: "at home all weekend"},</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
@@ -2967,32 +3351,32 @@
         <v>0</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>16</v>
+        <v>188</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>2</v>
+        <v>189</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>4</v>
+        <v>190</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J80" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
+        <f>A80&amp;B80&amp;C80&amp;D80&amp;E80&amp;F80&amp;G80&amp;H80&amp;I80</f>
+        <v>{beginning: "He", bold: "feel", correct: "was feeling", ending: "bad about his decision"},</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
@@ -3000,32 +3384,32 @@
         <v>0</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>2</v>
+        <v>191</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>4</v>
+        <v>192</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J81" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" ref="J81:J86" si="7">A81&amp;B81&amp;C81&amp;D81&amp;E81&amp;F81&amp;G81&amp;H81&amp;I81</f>
+        <v>{beginning: "I", bold: "eat", correct: "was eating", ending: "the cake when they arrived"},</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
@@ -3033,67 +3417,131 @@
         <v>0</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>18</v>
+        <v>193</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>4</v>
+        <v>195</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J82" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="7"/>
+        <v>{beginning: "We", bold: "discuss", correct: "were discussing", ending: "the theory in the class"},</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J83" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>{beginning: "She", bold: "prepare", correct: "was preparing", ending: "dinner for her friends"},</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A84" s="4" t="s">
-        <v>25</v>
+      <c r="A84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J84" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>{beginning: "The students", bold: "study", correct: "were studying", ending: "law all evening"},</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B85" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="C85" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>8</v>
+        <v>203</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>9</v>
+        <v>204</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>10</v>
+        <v>205</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J85" s="2" t="str">
-        <f>A85&amp;B85&amp;C85&amp;D85&amp;E85&amp;F85&amp;G85&amp;H85&amp;I85</f>
-        <v>{beginning: "", bold: "Я", correct: "I", ending: "love Ukraine"},</v>
+        <f t="shared" si="7"/>
+        <v>{beginning: "She", bold: "cook", correct: "was cooking", ending: "food when I called"},</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
@@ -3101,98 +3549,37 @@
         <v>0</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>1</v>
+        <v>206</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>6</v>
+        <v>207</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>2</v>
+        <v>208</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>4</v>
+        <v>209</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J86" s="2" t="str">
-        <f>A86&amp;B86&amp;C86&amp;D86&amp;E86&amp;F86&amp;G86&amp;H86&amp;I86</f>
-        <v>{beginning: "beginning text", bold: "word text2", correct: "translate text", ending: "ending text"},</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H87" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I87" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J87" s="2" t="str">
-        <f t="shared" ref="J87:J94" si="7">A87&amp;B87&amp;C87&amp;D87&amp;E87&amp;F87&amp;G87&amp;H87&amp;I87</f>
-        <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="7"/>
+        <v>{beginning: "The boys", bold: "put", correct: "were putting", ending: "the books on the shelf"},</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H88" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I88" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J88" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
+      <c r="A88" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
@@ -3200,32 +3587,32 @@
         <v>0</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>13</v>
+        <v>210</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>2</v>
+        <v>211</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>4</v>
+        <v>212</v>
       </c>
       <c r="I89" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J89" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
+        <f>A89&amp;B89&amp;C89&amp;D89&amp;E89&amp;F89&amp;G89&amp;H89&amp;I89</f>
+        <v>{beginning: "The bird", bold: "sing (past)", correct: "was not singing", ending: "in the morning"},</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
@@ -3233,32 +3620,32 @@
         <v>0</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>1</v>
+        <v>213</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>4</v>
+        <v>216</v>
       </c>
       <c r="I90" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J90" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
+        <f>A90&amp;B90&amp;C90&amp;D90&amp;E90&amp;F90&amp;G90&amp;H90&amp;I90</f>
+        <v>{beginning: "The guide", bold: "explain (present)", correct: "is not explaining", ending: "it clearly"},</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
@@ -3266,32 +3653,32 @@
         <v>0</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>15</v>
+        <v>217</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>2</v>
+        <v>218</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>4</v>
+        <v>219</v>
       </c>
       <c r="I91" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J91" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" ref="J91:J96" si="8">A91&amp;B91&amp;C91&amp;D91&amp;E91&amp;F91&amp;G91&amp;H91&amp;I91</f>
+        <v>{beginning: "They", bold: "provide (future)", correct: "will not be providing", ending: "enough information"},</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
@@ -3299,32 +3686,32 @@
         <v>0</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>16</v>
+        <v>220</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>2</v>
+        <v>221</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>4</v>
+        <v>222</v>
       </c>
       <c r="I92" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J92" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="8"/>
+        <v>{beginning: "She", bold: "change (past)", correct: "was not changing", ending: "her opinion"},</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
@@ -3332,32 +3719,32 @@
         <v>0</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>17</v>
+        <v>223</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>2</v>
+        <v>224</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="I93" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J93" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="8"/>
+        <v>{beginning: "He", bold: "show (future)", correct: "will not be showing", ending: "interest in this topic"},</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
@@ -3365,100 +3752,103 @@
         <v>0</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>18</v>
+        <v>226</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>2</v>
+        <v>227</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>4</v>
+        <v>228</v>
       </c>
       <c r="I94" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J94" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="8"/>
+        <v>{beginning: "We", bold: "study (present)", correct: "are not studying", ending: "literature at this lesson"},</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J95" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>{beginning: "I", bold: "visit (past)", correct: "was not visiting", ending: "them last month"},</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A96" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H97" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I97" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J97" s="2" t="str">
-        <f>A97&amp;B97&amp;C97&amp;D97&amp;E97&amp;F97&amp;G97&amp;H97&amp;I97</f>
-        <v>{beginning: "", bold: "Я", correct: "I", ending: "love Ukraine"},</v>
+      <c r="A96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J96" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>{beginning: "They", bold: "solve (future)", correct: "will not be solving", ending: "the problem correctly"},</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H98" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J98" s="2" t="str">
-        <f>A98&amp;B98&amp;C98&amp;D98&amp;E98&amp;F98&amp;G98&amp;H98&amp;I98</f>
-        <v>{beginning: "beginning text", bold: "word text2", correct: "translate text", ending: "ending text"},</v>
+      <c r="A98" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
@@ -3466,32 +3856,32 @@
         <v>0</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>2</v>
+        <v>235</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>4</v>
+        <v>236</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J99" s="2" t="str">
-        <f t="shared" ref="J99:J106" si="8">A99&amp;B99&amp;C99&amp;D99&amp;E99&amp;F99&amp;G99&amp;H99&amp;I99</f>
-        <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
+        <f>A99&amp;B99&amp;C99&amp;D99&amp;E99&amp;F99&amp;G99&amp;H99&amp;I99</f>
+        <v>{beginning: "She", bold: "find", correct: "has not found", ending: "her card"},</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
@@ -3499,32 +3889,32 @@
         <v>0</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>12</v>
+        <v>237</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>2</v>
+        <v>238</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>4</v>
+        <v>239</v>
       </c>
       <c r="I100" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J100" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
+        <f>A100&amp;B100&amp;C100&amp;D100&amp;E100&amp;F100&amp;G100&amp;H100&amp;I100</f>
+        <v>{beginning: "They", bold: "face", correct: "have not faced", ending: "any difficulties so far"},</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
@@ -3532,32 +3922,32 @@
         <v>0</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>13</v>
+        <v>240</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>2</v>
+        <v>241</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>4</v>
+        <v>242</v>
       </c>
       <c r="I101" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J101" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" ref="J101:J106" si="9">A101&amp;B101&amp;C101&amp;D101&amp;E101&amp;F101&amp;G101&amp;H101&amp;I101</f>
+        <v>{beginning: "We", bold: "include", correct: "have not included", ending: "Sarah in the list"},</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
@@ -3565,32 +3955,32 @@
         <v>0</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>2</v>
+        <v>243</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>4</v>
+        <v>244</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J102" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="9"/>
+        <v>{beginning: "He", bold: "make", correct: "has not made", ending: "a list of items to buy"},</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
@@ -3598,32 +3988,32 @@
         <v>0</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>2</v>
+        <v>245</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>4</v>
+        <v>246</v>
       </c>
       <c r="I103" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J103" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="9"/>
+        <v>{beginning: "I", bold: "change", correct: "have not changed", ending: "my mind about the trip"},</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
@@ -3631,32 +4021,32 @@
         <v>0</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>16</v>
+        <v>247</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>2</v>
+        <v>248</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>4</v>
+        <v>249</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J104" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="9"/>
+        <v>{beginning: "She", bold: "mention", correct: "has not mentioned", ending: "any reason"},</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
@@ -3664,32 +4054,32 @@
         <v>0</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>17</v>
+        <v>250</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>2</v>
+        <v>251</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>4</v>
+        <v>252</v>
       </c>
       <c r="I105" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J105" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="9"/>
+        <v>{beginning: "You", bold: "see", correct: "have not seen", ending: "the real problem yet"},</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
@@ -3697,37 +4087,37 @@
         <v>0</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>2</v>
+        <v>254</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>4</v>
+        <v>255</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J106" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
+        <f t="shared" si="9"/>
+        <v>{beginning: "I", bold: "try", correct: "have not tried", ending: "various solutions yet"},</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
@@ -3822,7 +4212,7 @@
         <v>5</v>
       </c>
       <c r="J111" s="2" t="str">
-        <f t="shared" ref="J111:J118" si="9">A111&amp;B111&amp;C111&amp;D111&amp;E111&amp;F111&amp;G111&amp;H111&amp;I111</f>
+        <f t="shared" ref="J111:J118" si="10">A111&amp;B111&amp;C111&amp;D111&amp;E111&amp;F111&amp;G111&amp;H111&amp;I111</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -3855,7 +4245,7 @@
         <v>5</v>
       </c>
       <c r="J112" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -3888,7 +4278,7 @@
         <v>5</v>
       </c>
       <c r="J113" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -3921,7 +4311,7 @@
         <v>5</v>
       </c>
       <c r="J114" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -3954,7 +4344,7 @@
         <v>5</v>
       </c>
       <c r="J115" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -3987,7 +4377,7 @@
         <v>5</v>
       </c>
       <c r="J116" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4020,7 +4410,7 @@
         <v>5</v>
       </c>
       <c r="J117" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4053,13 +4443,13 @@
         <v>5</v>
       </c>
       <c r="J118" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.3">
@@ -4154,7 +4544,7 @@
         <v>5</v>
       </c>
       <c r="J123" s="2" t="str">
-        <f t="shared" ref="J123:J130" si="10">A123&amp;B123&amp;C123&amp;D123&amp;E123&amp;F123&amp;G123&amp;H123&amp;I123</f>
+        <f t="shared" ref="J123:J130" si="11">A123&amp;B123&amp;C123&amp;D123&amp;E123&amp;F123&amp;G123&amp;H123&amp;I123</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4187,7 +4577,7 @@
         <v>5</v>
       </c>
       <c r="J124" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4220,7 +4610,7 @@
         <v>5</v>
       </c>
       <c r="J125" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4253,7 +4643,7 @@
         <v>5</v>
       </c>
       <c r="J126" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4286,7 +4676,7 @@
         <v>5</v>
       </c>
       <c r="J127" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4319,7 +4709,7 @@
         <v>5</v>
       </c>
       <c r="J128" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4352,7 +4742,7 @@
         <v>5</v>
       </c>
       <c r="J129" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4385,13 +4775,13 @@
         <v>5</v>
       </c>
       <c r="J130" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.3">
@@ -4486,7 +4876,7 @@
         <v>5</v>
       </c>
       <c r="J135" s="2" t="str">
-        <f t="shared" ref="J135:J142" si="11">A135&amp;B135&amp;C135&amp;D135&amp;E135&amp;F135&amp;G135&amp;H135&amp;I135</f>
+        <f t="shared" ref="J135:J142" si="12">A135&amp;B135&amp;C135&amp;D135&amp;E135&amp;F135&amp;G135&amp;H135&amp;I135</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4519,7 +4909,7 @@
         <v>5</v>
       </c>
       <c r="J136" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4552,7 +4942,7 @@
         <v>5</v>
       </c>
       <c r="J137" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4585,7 +4975,7 @@
         <v>5</v>
       </c>
       <c r="J138" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4618,7 +5008,7 @@
         <v>5</v>
       </c>
       <c r="J139" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4651,7 +5041,7 @@
         <v>5</v>
       </c>
       <c r="J140" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4684,7 +5074,7 @@
         <v>5</v>
       </c>
       <c r="J141" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4717,13 +5107,13 @@
         <v>5</v>
       </c>
       <c r="J142" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.3">
@@ -4818,7 +5208,7 @@
         <v>5</v>
       </c>
       <c r="J147" s="2" t="str">
-        <f t="shared" ref="J147:J154" si="12">A147&amp;B147&amp;C147&amp;D147&amp;E147&amp;F147&amp;G147&amp;H147&amp;I147</f>
+        <f t="shared" ref="J147:J154" si="13">A147&amp;B147&amp;C147&amp;D147&amp;E147&amp;F147&amp;G147&amp;H147&amp;I147</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4851,7 +5241,7 @@
         <v>5</v>
       </c>
       <c r="J148" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4884,7 +5274,7 @@
         <v>5</v>
       </c>
       <c r="J149" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4917,7 +5307,7 @@
         <v>5</v>
       </c>
       <c r="J150" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4950,7 +5340,7 @@
         <v>5</v>
       </c>
       <c r="J151" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -4983,7 +5373,7 @@
         <v>5</v>
       </c>
       <c r="J152" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5016,7 +5406,7 @@
         <v>5</v>
       </c>
       <c r="J153" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5049,13 +5439,13 @@
         <v>5</v>
       </c>
       <c r="J154" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A156" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.3">
@@ -5150,7 +5540,7 @@
         <v>5</v>
       </c>
       <c r="J159" s="2" t="str">
-        <f t="shared" ref="J159:J166" si="13">A159&amp;B159&amp;C159&amp;D159&amp;E159&amp;F159&amp;G159&amp;H159&amp;I159</f>
+        <f t="shared" ref="J159:J166" si="14">A159&amp;B159&amp;C159&amp;D159&amp;E159&amp;F159&amp;G159&amp;H159&amp;I159</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5183,7 +5573,7 @@
         <v>5</v>
       </c>
       <c r="J160" s="2" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5216,7 +5606,7 @@
         <v>5</v>
       </c>
       <c r="J161" s="2" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5249,7 +5639,7 @@
         <v>5</v>
       </c>
       <c r="J162" s="2" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5282,7 +5672,7 @@
         <v>5</v>
       </c>
       <c r="J163" s="2" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5315,7 +5705,7 @@
         <v>5</v>
       </c>
       <c r="J164" s="2" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5348,7 +5738,7 @@
         <v>5</v>
       </c>
       <c r="J165" s="2" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5381,13 +5771,13 @@
         <v>5</v>
       </c>
       <c r="J166" s="2" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A168" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.3">
@@ -5482,7 +5872,7 @@
         <v>5</v>
       </c>
       <c r="J171" s="2" t="str">
-        <f t="shared" ref="J171:J178" si="14">A171&amp;B171&amp;C171&amp;D171&amp;E171&amp;F171&amp;G171&amp;H171&amp;I171</f>
+        <f t="shared" ref="J171:J178" si="15">A171&amp;B171&amp;C171&amp;D171&amp;E171&amp;F171&amp;G171&amp;H171&amp;I171</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5515,7 +5905,7 @@
         <v>5</v>
       </c>
       <c r="J172" s="2" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5548,7 +5938,7 @@
         <v>5</v>
       </c>
       <c r="J173" s="2" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5581,7 +5971,7 @@
         <v>5</v>
       </c>
       <c r="J174" s="2" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5614,7 +6004,7 @@
         <v>5</v>
       </c>
       <c r="J175" s="2" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5647,7 +6037,7 @@
         <v>5</v>
       </c>
       <c r="J176" s="2" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5680,7 +6070,7 @@
         <v>5</v>
       </c>
       <c r="J177" s="2" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5713,13 +6103,13 @@
         <v>5</v>
       </c>
       <c r="J178" s="2" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A180" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.3">
@@ -5814,7 +6204,7 @@
         <v>5</v>
       </c>
       <c r="J183" s="2" t="str">
-        <f t="shared" ref="J183:J190" si="15">A183&amp;B183&amp;C183&amp;D183&amp;E183&amp;F183&amp;G183&amp;H183&amp;I183</f>
+        <f t="shared" ref="J183:J190" si="16">A183&amp;B183&amp;C183&amp;D183&amp;E183&amp;F183&amp;G183&amp;H183&amp;I183</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5847,7 +6237,7 @@
         <v>5</v>
       </c>
       <c r="J184" s="2" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5880,7 +6270,7 @@
         <v>5</v>
       </c>
       <c r="J185" s="2" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5913,7 +6303,7 @@
         <v>5</v>
       </c>
       <c r="J186" s="2" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5946,7 +6336,7 @@
         <v>5</v>
       </c>
       <c r="J187" s="2" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -5979,7 +6369,7 @@
         <v>5</v>
       </c>
       <c r="J188" s="2" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6012,7 +6402,7 @@
         <v>5</v>
       </c>
       <c r="J189" s="2" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6045,13 +6435,13 @@
         <v>5</v>
       </c>
       <c r="J190" s="2" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A192" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.3">
@@ -6146,7 +6536,7 @@
         <v>5</v>
       </c>
       <c r="J195" s="2" t="str">
-        <f t="shared" ref="J195:J202" si="16">A195&amp;B195&amp;C195&amp;D195&amp;E195&amp;F195&amp;G195&amp;H195&amp;I195</f>
+        <f t="shared" ref="J195:J202" si="17">A195&amp;B195&amp;C195&amp;D195&amp;E195&amp;F195&amp;G195&amp;H195&amp;I195</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6179,7 +6569,7 @@
         <v>5</v>
       </c>
       <c r="J196" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6212,7 +6602,7 @@
         <v>5</v>
       </c>
       <c r="J197" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6245,7 +6635,7 @@
         <v>5</v>
       </c>
       <c r="J198" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6278,7 +6668,7 @@
         <v>5</v>
       </c>
       <c r="J199" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6311,7 +6701,7 @@
         <v>5</v>
       </c>
       <c r="J200" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6344,7 +6734,7 @@
         <v>5</v>
       </c>
       <c r="J201" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6377,13 +6767,13 @@
         <v>5</v>
       </c>
       <c r="J202" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A204" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.3">
@@ -6478,7 +6868,7 @@
         <v>5</v>
       </c>
       <c r="J207" s="2" t="str">
-        <f t="shared" ref="J207:J214" si="17">A207&amp;B207&amp;C207&amp;D207&amp;E207&amp;F207&amp;G207&amp;H207&amp;I207</f>
+        <f t="shared" ref="J207:J214" si="18">A207&amp;B207&amp;C207&amp;D207&amp;E207&amp;F207&amp;G207&amp;H207&amp;I207</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6511,7 +6901,7 @@
         <v>5</v>
       </c>
       <c r="J208" s="2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6544,7 +6934,7 @@
         <v>5</v>
       </c>
       <c r="J209" s="2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6577,7 +6967,7 @@
         <v>5</v>
       </c>
       <c r="J210" s="2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6610,7 +7000,7 @@
         <v>5</v>
       </c>
       <c r="J211" s="2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6643,7 +7033,7 @@
         <v>5</v>
       </c>
       <c r="J212" s="2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6676,7 +7066,7 @@
         <v>5</v>
       </c>
       <c r="J213" s="2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6709,13 +7099,13 @@
         <v>5</v>
       </c>
       <c r="J214" s="2" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A216" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.3">
@@ -6810,7 +7200,7 @@
         <v>5</v>
       </c>
       <c r="J219" s="2" t="str">
-        <f t="shared" ref="J219:J226" si="18">A219&amp;B219&amp;C219&amp;D219&amp;E219&amp;F219&amp;G219&amp;H219&amp;I219</f>
+        <f t="shared" ref="J219:J226" si="19">A219&amp;B219&amp;C219&amp;D219&amp;E219&amp;F219&amp;G219&amp;H219&amp;I219</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6843,7 +7233,7 @@
         <v>5</v>
       </c>
       <c r="J220" s="2" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6876,7 +7266,7 @@
         <v>5</v>
       </c>
       <c r="J221" s="2" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6909,7 +7299,7 @@
         <v>5</v>
       </c>
       <c r="J222" s="2" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6942,7 +7332,7 @@
         <v>5</v>
       </c>
       <c r="J223" s="2" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -6975,7 +7365,7 @@
         <v>5</v>
       </c>
       <c r="J224" s="2" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7008,7 +7398,7 @@
         <v>5</v>
       </c>
       <c r="J225" s="2" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7041,13 +7431,13 @@
         <v>5</v>
       </c>
       <c r="J226" s="2" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A228" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.3">
@@ -7142,7 +7532,7 @@
         <v>5</v>
       </c>
       <c r="J231" s="2" t="str">
-        <f t="shared" ref="J231:J238" si="19">A231&amp;B231&amp;C231&amp;D231&amp;E231&amp;F231&amp;G231&amp;H231&amp;I231</f>
+        <f t="shared" ref="J231:J238" si="20">A231&amp;B231&amp;C231&amp;D231&amp;E231&amp;F231&amp;G231&amp;H231&amp;I231</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7175,7 +7565,7 @@
         <v>5</v>
       </c>
       <c r="J232" s="2" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7208,7 +7598,7 @@
         <v>5</v>
       </c>
       <c r="J233" s="2" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7241,7 +7631,7 @@
         <v>5</v>
       </c>
       <c r="J234" s="2" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7274,7 +7664,7 @@
         <v>5</v>
       </c>
       <c r="J235" s="2" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7307,7 +7697,7 @@
         <v>5</v>
       </c>
       <c r="J236" s="2" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7340,7 +7730,7 @@
         <v>5</v>
       </c>
       <c r="J237" s="2" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7373,13 +7763,13 @@
         <v>5</v>
       </c>
       <c r="J238" s="2" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A240" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.3">
@@ -7474,7 +7864,7 @@
         <v>5</v>
       </c>
       <c r="J243" s="2" t="str">
-        <f t="shared" ref="J243:J250" si="20">A243&amp;B243&amp;C243&amp;D243&amp;E243&amp;F243&amp;G243&amp;H243&amp;I243</f>
+        <f t="shared" ref="J243:J250" si="21">A243&amp;B243&amp;C243&amp;D243&amp;E243&amp;F243&amp;G243&amp;H243&amp;I243</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7507,7 +7897,7 @@
         <v>5</v>
       </c>
       <c r="J244" s="2" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7540,7 +7930,7 @@
         <v>5</v>
       </c>
       <c r="J245" s="2" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7573,7 +7963,7 @@
         <v>5</v>
       </c>
       <c r="J246" s="2" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7606,7 +7996,7 @@
         <v>5</v>
       </c>
       <c r="J247" s="2" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7639,7 +8029,7 @@
         <v>5</v>
       </c>
       <c r="J248" s="2" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7672,7 +8062,7 @@
         <v>5</v>
       </c>
       <c r="J249" s="2" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7705,13 +8095,13 @@
         <v>5</v>
       </c>
       <c r="J250" s="2" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A252" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.3">
@@ -7806,7 +8196,7 @@
         <v>5</v>
       </c>
       <c r="J255" s="2" t="str">
-        <f t="shared" ref="J255:J262" si="21">A255&amp;B255&amp;C255&amp;D255&amp;E255&amp;F255&amp;G255&amp;H255&amp;I255</f>
+        <f t="shared" ref="J255:J262" si="22">A255&amp;B255&amp;C255&amp;D255&amp;E255&amp;F255&amp;G255&amp;H255&amp;I255</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7839,7 +8229,7 @@
         <v>5</v>
       </c>
       <c r="J256" s="2" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7872,7 +8262,7 @@
         <v>5</v>
       </c>
       <c r="J257" s="2" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7905,7 +8295,7 @@
         <v>5</v>
       </c>
       <c r="J258" s="2" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7938,7 +8328,7 @@
         <v>5</v>
       </c>
       <c r="J259" s="2" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -7971,7 +8361,7 @@
         <v>5</v>
       </c>
       <c r="J260" s="2" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8004,7 +8394,7 @@
         <v>5</v>
       </c>
       <c r="J261" s="2" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8037,13 +8427,13 @@
         <v>5</v>
       </c>
       <c r="J262" s="2" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A264" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.3">
@@ -8138,7 +8528,7 @@
         <v>5</v>
       </c>
       <c r="J267" s="2" t="str">
-        <f t="shared" ref="J267:J274" si="22">A267&amp;B267&amp;C267&amp;D267&amp;E267&amp;F267&amp;G267&amp;H267&amp;I267</f>
+        <f t="shared" ref="J267:J274" si="23">A267&amp;B267&amp;C267&amp;D267&amp;E267&amp;F267&amp;G267&amp;H267&amp;I267</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8171,7 +8561,7 @@
         <v>5</v>
       </c>
       <c r="J268" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8204,7 +8594,7 @@
         <v>5</v>
       </c>
       <c r="J269" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8237,7 +8627,7 @@
         <v>5</v>
       </c>
       <c r="J270" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8270,7 +8660,7 @@
         <v>5</v>
       </c>
       <c r="J271" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8303,7 +8693,7 @@
         <v>5</v>
       </c>
       <c r="J272" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8336,7 +8726,7 @@
         <v>5</v>
       </c>
       <c r="J273" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8369,13 +8759,13 @@
         <v>5</v>
       </c>
       <c r="J274" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A276" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.3">
@@ -8470,7 +8860,7 @@
         <v>5</v>
       </c>
       <c r="J279" s="2" t="str">
-        <f t="shared" ref="J279:J286" si="23">A279&amp;B279&amp;C279&amp;D279&amp;E279&amp;F279&amp;G279&amp;H279&amp;I279</f>
+        <f t="shared" ref="J279:J286" si="24">A279&amp;B279&amp;C279&amp;D279&amp;E279&amp;F279&amp;G279&amp;H279&amp;I279</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8503,7 +8893,7 @@
         <v>5</v>
       </c>
       <c r="J280" s="2" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8536,7 +8926,7 @@
         <v>5</v>
       </c>
       <c r="J281" s="2" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8569,7 +8959,7 @@
         <v>5</v>
       </c>
       <c r="J282" s="2" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8602,7 +8992,7 @@
         <v>5</v>
       </c>
       <c r="J283" s="2" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8635,7 +9025,7 @@
         <v>5</v>
       </c>
       <c r="J284" s="2" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8668,7 +9058,7 @@
         <v>5</v>
       </c>
       <c r="J285" s="2" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8701,13 +9091,13 @@
         <v>5</v>
       </c>
       <c r="J286" s="2" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="288" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A288" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.3">
@@ -8802,7 +9192,7 @@
         <v>5</v>
       </c>
       <c r="J291" s="2" t="str">
-        <f t="shared" ref="J291:J298" si="24">A291&amp;B291&amp;C291&amp;D291&amp;E291&amp;F291&amp;G291&amp;H291&amp;I291</f>
+        <f t="shared" ref="J291:J298" si="25">A291&amp;B291&amp;C291&amp;D291&amp;E291&amp;F291&amp;G291&amp;H291&amp;I291</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8835,7 +9225,7 @@
         <v>5</v>
       </c>
       <c r="J292" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8868,7 +9258,7 @@
         <v>5</v>
       </c>
       <c r="J293" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8901,7 +9291,7 @@
         <v>5</v>
       </c>
       <c r="J294" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8934,7 +9324,7 @@
         <v>5</v>
       </c>
       <c r="J295" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -8967,7 +9357,7 @@
         <v>5</v>
       </c>
       <c r="J296" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9000,7 +9390,7 @@
         <v>5</v>
       </c>
       <c r="J297" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9033,13 +9423,13 @@
         <v>5</v>
       </c>
       <c r="J298" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A300" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.3">
@@ -9134,7 +9524,7 @@
         <v>5</v>
       </c>
       <c r="J303" s="2" t="str">
-        <f t="shared" ref="J303:J310" si="25">A303&amp;B303&amp;C303&amp;D303&amp;E303&amp;F303&amp;G303&amp;H303&amp;I303</f>
+        <f t="shared" ref="J303:J310" si="26">A303&amp;B303&amp;C303&amp;D303&amp;E303&amp;F303&amp;G303&amp;H303&amp;I303</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9167,7 +9557,7 @@
         <v>5</v>
       </c>
       <c r="J304" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9200,7 +9590,7 @@
         <v>5</v>
       </c>
       <c r="J305" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9233,7 +9623,7 @@
         <v>5</v>
       </c>
       <c r="J306" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9266,7 +9656,7 @@
         <v>5</v>
       </c>
       <c r="J307" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9299,7 +9689,7 @@
         <v>5</v>
       </c>
       <c r="J308" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9332,7 +9722,7 @@
         <v>5</v>
       </c>
       <c r="J309" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9365,13 +9755,13 @@
         <v>5</v>
       </c>
       <c r="J310" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="312" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A312" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="313" spans="1:10" x14ac:dyDescent="0.3">
@@ -9466,7 +9856,7 @@
         <v>5</v>
       </c>
       <c r="J315" s="2" t="str">
-        <f t="shared" ref="J315:J322" si="26">A315&amp;B315&amp;C315&amp;D315&amp;E315&amp;F315&amp;G315&amp;H315&amp;I315</f>
+        <f t="shared" ref="J315:J322" si="27">A315&amp;B315&amp;C315&amp;D315&amp;E315&amp;F315&amp;G315&amp;H315&amp;I315</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9499,7 +9889,7 @@
         <v>5</v>
       </c>
       <c r="J316" s="2" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9532,7 +9922,7 @@
         <v>5</v>
       </c>
       <c r="J317" s="2" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9565,7 +9955,7 @@
         <v>5</v>
       </c>
       <c r="J318" s="2" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9598,7 +9988,7 @@
         <v>5</v>
       </c>
       <c r="J319" s="2" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9631,7 +10021,7 @@
         <v>5</v>
       </c>
       <c r="J320" s="2" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9664,7 +10054,7 @@
         <v>5</v>
       </c>
       <c r="J321" s="2" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9697,13 +10087,13 @@
         <v>5</v>
       </c>
       <c r="J322" s="2" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="324" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A324" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="325" spans="1:10" x14ac:dyDescent="0.3">
@@ -9798,7 +10188,7 @@
         <v>5</v>
       </c>
       <c r="J327" s="2" t="str">
-        <f t="shared" ref="J327:J334" si="27">A327&amp;B327&amp;C327&amp;D327&amp;E327&amp;F327&amp;G327&amp;H327&amp;I327</f>
+        <f t="shared" ref="J327:J334" si="28">A327&amp;B327&amp;C327&amp;D327&amp;E327&amp;F327&amp;G327&amp;H327&amp;I327</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9831,7 +10221,7 @@
         <v>5</v>
       </c>
       <c r="J328" s="2" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9864,7 +10254,7 @@
         <v>5</v>
       </c>
       <c r="J329" s="2" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9897,7 +10287,7 @@
         <v>5</v>
       </c>
       <c r="J330" s="2" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9930,7 +10320,7 @@
         <v>5</v>
       </c>
       <c r="J331" s="2" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9963,7 +10353,7 @@
         <v>5</v>
       </c>
       <c r="J332" s="2" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -9996,7 +10386,7 @@
         <v>5</v>
       </c>
       <c r="J333" s="2" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -10029,13 +10419,13 @@
         <v>5</v>
       </c>
       <c r="J334" s="2" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
     <row r="336" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A336" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="337" spans="1:10" x14ac:dyDescent="0.3">
@@ -10130,7 +10520,7 @@
         <v>5</v>
       </c>
       <c r="J339" s="2" t="str">
-        <f t="shared" ref="J339:J346" si="28">A339&amp;B339&amp;C339&amp;D339&amp;E339&amp;F339&amp;G339&amp;H339&amp;I339</f>
+        <f t="shared" ref="J339:J346" si="29">A339&amp;B339&amp;C339&amp;D339&amp;E339&amp;F339&amp;G339&amp;H339&amp;I339</f>
         <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -10163,7 +10553,7 @@
         <v>5</v>
       </c>
       <c r="J340" s="2" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -10196,7 +10586,7 @@
         <v>5</v>
       </c>
       <c r="J341" s="2" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -10229,7 +10619,7 @@
         <v>5</v>
       </c>
       <c r="J342" s="2" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -10262,7 +10652,7 @@
         <v>5</v>
       </c>
       <c r="J343" s="2" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -10295,7 +10685,7 @@
         <v>5</v>
       </c>
       <c r="J344" s="2" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -10328,7 +10718,7 @@
         <v>5</v>
       </c>
       <c r="J345" s="2" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
       </c>
     </row>
@@ -10361,338 +10751,6 @@
         <v>5</v>
       </c>
       <c r="J346" s="2" t="str">
-        <f t="shared" si="28"/>
-        <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
-      </c>
-    </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A348" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A349" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C349" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D349" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E349" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F349" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G349" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H349" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I349" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J349" s="2" t="str">
-        <f>A349&amp;B349&amp;C349&amp;D349&amp;E349&amp;F349&amp;G349&amp;H349&amp;I349</f>
-        <v>{beginning: "", bold: "Я", correct: "I", ending: "love Ukraine"},</v>
-      </c>
-    </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A350" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B350" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C350" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D350" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E350" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F350" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G350" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H350" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I350" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J350" s="2" t="str">
-        <f>A350&amp;B350&amp;C350&amp;D350&amp;E350&amp;F350&amp;G350&amp;H350&amp;I350</f>
-        <v>{beginning: "beginning text", bold: "word text2", correct: "translate text", ending: "ending text"},</v>
-      </c>
-    </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A351" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B351" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C351" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D351" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E351" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F351" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G351" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H351" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I351" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J351" s="2" t="str">
-        <f t="shared" ref="J351:J358" si="29">A351&amp;B351&amp;C351&amp;D351&amp;E351&amp;F351&amp;G351&amp;H351&amp;I351</f>
-        <v>{beginning: "beginning text", bold: "word text3", correct: "translate text", ending: "ending text"},</v>
-      </c>
-    </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A352" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B352" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C352" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D352" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E352" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F352" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G352" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H352" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I352" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J352" s="2" t="str">
-        <f t="shared" si="29"/>
-        <v>{beginning: "beginning text", bold: "word text4", correct: "translate text", ending: "ending text"},</v>
-      </c>
-    </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A353" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B353" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C353" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D353" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E353" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F353" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G353" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H353" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I353" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J353" s="2" t="str">
-        <f t="shared" si="29"/>
-        <v>{beginning: "beginning text", bold: "word text5", correct: "translate text", ending: "ending text"},</v>
-      </c>
-    </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A354" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B354" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C354" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D354" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E354" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F354" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G354" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H354" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I354" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J354" s="2" t="str">
-        <f t="shared" si="29"/>
-        <v>{beginning: "beginning text", bold: "word text6", correct: "translate text", ending: "ending text"},</v>
-      </c>
-    </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A355" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B355" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C355" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D355" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E355" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F355" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G355" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H355" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I355" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J355" s="2" t="str">
-        <f t="shared" si="29"/>
-        <v>{beginning: "beginning text", bold: "word text7", correct: "translate text", ending: "ending text"},</v>
-      </c>
-    </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A356" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B356" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C356" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D356" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E356" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F356" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G356" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H356" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I356" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J356" s="2" t="str">
-        <f t="shared" si="29"/>
-        <v>{beginning: "beginning text", bold: "word text8", correct: "translate text", ending: "ending text"},</v>
-      </c>
-    </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A357" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B357" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C357" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D357" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E357" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F357" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G357" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H357" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I357" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J357" s="2" t="str">
-        <f t="shared" si="29"/>
-        <v>{beginning: "beginning text", bold: "word text9", correct: "translate text", ending: "ending text"},</v>
-      </c>
-    </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A358" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B358" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C358" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D358" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E358" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F358" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G358" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H358" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I358" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J358" s="2" t="str">
         <f t="shared" si="29"/>
         <v>{beginning: "beginning text", bold: "word text10", correct: "translate text", ending: "ending text"},</v>
       </c>

</xml_diff>